<commit_message>
added demo test files
</commit_message>
<xml_diff>
--- a/Demo/TestData/data.xlsx
+++ b/Demo/TestData/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mobile Programming\eclipse-workspace\Demo\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\backup\Git\demo\Demo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17196" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -31,6 +31,15 @@
   </si>
   <si>
     <t>rahaguh</t>
+  </si>
+  <si>
+    <t>rahjjjjjaguh</t>
+  </si>
+  <si>
+    <t>mngr429679</t>
+  </si>
+  <si>
+    <t>jYdyvYg</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -310,18 +319,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -329,7 +338,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>